<commit_message>
Updated data config for auto_retry asset
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Kalyana\#_Email\Traveloka_DataAutomation_Performer_Email\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 1\Traveloka_DataAutomation_Performer_Email_S1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D099BF5-6ABE-4C76-8EBC-09AACB0EFAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAA8A55-BA93-4643-AF7C-689005660FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +196,30 @@
   </si>
   <si>
     <t>RPA_Moon_SenderName</t>
+  </si>
+  <si>
+    <t>AutoRetryMax</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryMax</t>
+  </si>
+  <si>
+    <t>AutoRetryPostpone</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryPostpone</t>
+  </si>
+  <si>
+    <t>AutoRetryMaxDay</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryMaxDay</t>
+  </si>
+  <si>
+    <t>AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetrySchedule</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +2870,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2909,10 +2933,38 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>